<commit_message>
Update ASTM list with new RT and plotly confirmation of overlapping of RT1 and RT2 between ASTM and aligned compounds
</commit_message>
<xml_diff>
--- a/ASTM Compound List.xlsx
+++ b/ASTM Compound List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ryersonprod-my.sharepoint.com/personal/huy_manh_nguyen_ryerson_ca/Documents/Huy Nguyen/PhD_EnSciMan_TMU/Arson project/Rproject/Arson/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{451FB2BB-1E18-43AA-9341-05288591136D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AD90150-8C73-4EB8-9565-A7D282B8A6AA}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{451FB2BB-1E18-43AA-9341-05288591136D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98FCD6C4-B76A-4960-AB7F-7BAE9CDE07B5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -350,6 +350,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -642,7 +646,7 @@
   <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:X1048576"/>
+      <selection activeCell="E36" sqref="E36:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,7 +655,7 @@
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>